<commit_message>
add bottom caption & translation
</commit_message>
<xml_diff>
--- a/inst/extdata/label_translations.xlsx
+++ b/inst/extdata/label_translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Desktop\CREA Github\temp\china_co2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799F3364-C2BA-41C9-88BB-8545FC1A2C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB0CA6A-CF78-46C4-AC2C-45603AB06B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="915" windowWidth="19980" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8820" yWindow="885" windowWidth="19980" windowHeight="13935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="318">
   <si>
     <t>EN</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>PM2.5 concentrations in provincial capitals</t>
+  </si>
+  <si>
+    <t>数据截至</t>
+  </si>
+  <si>
+    <t>Data until</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1247,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B176"/>
+  <dimension ref="A1:B177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1253,7 +1259,7 @@
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="12.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="12.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1269,7 +1275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="12.75">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="12.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1285,7 +1291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="12.75">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="12.75">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" ht="12.75">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="12.75">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="12.75">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1325,7 +1331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="12.75">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1333,7 +1339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="12.75">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="12.75">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="12.75">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="12.75">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1365,7 +1371,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="12.75">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="12.75">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="12.75">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" ht="12.75">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1397,7 +1403,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="12.75">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="12.75">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="12.75">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="12.75">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1429,7 +1435,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="12.75">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="12.75">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="12.75">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -1453,7 +1459,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" ht="12.75">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" ht="12.75">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" ht="12.75">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" ht="12.75">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -1485,7 +1491,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" ht="12.75">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -1493,7 +1499,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" ht="12.75">
       <c r="A31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" ht="12.75">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1509,7 +1515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" ht="12.75">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" ht="12.75">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" ht="12.75">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" ht="12.75">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" ht="12.75">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" ht="12.75">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" ht="12.75">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" ht="12.75">
       <c r="A40" s="1" t="s">
         <v>78</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" ht="12.75">
       <c r="A41" s="1" t="s">
         <v>80</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" ht="12.75">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" ht="12.75">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" ht="12.75">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" ht="12.75">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" ht="12.75">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -1621,7 +1627,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" ht="12.75">
       <c r="A47" s="1" t="s">
         <v>92</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" ht="12.75">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="12.75">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" ht="12.75">
       <c r="A50" s="1" t="s">
         <v>98</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" ht="12.75">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" ht="12.75">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" ht="12.75">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" ht="12.75">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" ht="12.75">
       <c r="A55" s="1" t="s">
         <v>22</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" ht="12.75">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" ht="12.75">
       <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" ht="12.75">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
@@ -1717,7 +1723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" ht="12.75">
       <c r="A59" s="1" t="s">
         <v>113</v>
       </c>
@@ -1725,7 +1731,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" ht="12.75">
       <c r="A60" s="1" t="s">
         <v>115</v>
       </c>
@@ -1733,7 +1739,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" ht="12.75">
       <c r="A61" s="1" t="s">
         <v>117</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" ht="12.75">
       <c r="A62" s="1" t="s">
         <v>119</v>
       </c>
@@ -1749,7 +1755,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" ht="12.75">
       <c r="A63" s="1" t="s">
         <v>121</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" ht="12.75">
       <c r="A64" s="1" t="s">
         <v>123</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" ht="12.75">
       <c r="A65" s="1" t="s">
         <v>125</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" ht="12.75">
       <c r="A66" s="1" t="s">
         <v>127</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" ht="12.75">
       <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
@@ -1789,7 +1795,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" ht="12.75">
       <c r="A68" s="1" t="s">
         <v>131</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" ht="12.75">
       <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" ht="12.75">
       <c r="A70" s="1" t="s">
         <v>135</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" ht="12.75">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
@@ -1821,7 +1827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" ht="12.75">
       <c r="A72" s="1" t="s">
         <v>137</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" ht="12.75">
       <c r="A73" s="1" t="s">
         <v>139</v>
       </c>
@@ -1837,7 +1843,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" ht="12.75">
       <c r="A74" s="1" t="s">
         <v>141</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" ht="12.75">
       <c r="A75" s="1" t="s">
         <v>143</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" ht="12.75">
       <c r="A76" s="1" t="s">
         <v>145</v>
       </c>
@@ -1861,7 +1867,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" ht="12.75">
       <c r="A77" s="1" t="s">
         <v>147</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" ht="12.75">
       <c r="A78" s="1" t="s">
         <v>149</v>
       </c>
@@ -1877,7 +1883,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" ht="12.75">
       <c r="A79" s="1" t="s">
         <v>151</v>
       </c>
@@ -1885,7 +1891,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" ht="12.75">
       <c r="A80" s="1" t="s">
         <v>312</v>
       </c>
@@ -1893,7 +1899,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" ht="12.75">
       <c r="A81" s="1" t="s">
         <v>313</v>
       </c>
@@ -1901,7 +1907,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" ht="12.75">
       <c r="A82" s="1" t="s">
         <v>155</v>
       </c>
@@ -1909,7 +1915,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" ht="12.75">
       <c r="A83" s="1" t="s">
         <v>157</v>
       </c>
@@ -1917,7 +1923,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" ht="12.75">
       <c r="A84" s="1" t="s">
         <v>159</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" ht="12.75">
       <c r="A85" s="1" t="s">
         <v>161</v>
       </c>
@@ -1933,7 +1939,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" ht="12.75">
       <c r="A86" s="1" t="s">
         <v>163</v>
       </c>
@@ -1941,7 +1947,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" ht="12.75">
       <c r="A87" s="1" t="s">
         <v>165</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" ht="12.75">
       <c r="A88" s="1" t="s">
         <v>167</v>
       </c>
@@ -1957,7 +1963,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" ht="12.75">
       <c r="A89" s="1" t="s">
         <v>169</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" ht="12.75">
       <c r="A90" s="1" t="s">
         <v>171</v>
       </c>
@@ -1973,7 +1979,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" ht="12.75">
       <c r="A91" s="1" t="s">
         <v>173</v>
       </c>
@@ -1981,7 +1987,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" ht="12.75">
       <c r="A92" s="1" t="s">
         <v>175</v>
       </c>
@@ -1989,7 +1995,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" ht="12.75">
       <c r="A93" s="1" t="s">
         <v>177</v>
       </c>
@@ -1997,7 +2003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" ht="12.75">
       <c r="A94" s="1" t="s">
         <v>178</v>
       </c>
@@ -2005,7 +2011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" ht="12.75">
       <c r="A95" s="1" t="s">
         <v>179</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" ht="12.75">
       <c r="A96" s="1" t="s">
         <v>180</v>
       </c>
@@ -2021,7 +2027,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" ht="12.75">
       <c r="A97" s="1" t="s">
         <v>181</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" ht="12.75">
       <c r="A98" s="1" t="s">
         <v>182</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" ht="12.75">
       <c r="A99" s="1" t="s">
         <v>183</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" ht="12.75">
       <c r="A100" s="1" t="s">
         <v>185</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" ht="12.75">
       <c r="A101" s="1" t="s">
         <v>187</v>
       </c>
@@ -2061,7 +2067,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" ht="12.75">
       <c r="A102" s="1" t="s">
         <v>189</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" ht="12.75">
       <c r="A103" s="1" t="s">
         <v>191</v>
       </c>
@@ -2077,7 +2083,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" ht="12.75">
       <c r="A104" s="1" t="s">
         <v>193</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" ht="12.75">
       <c r="A105" s="1" t="s">
         <v>195</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" ht="12.75">
       <c r="A106" s="1" t="s">
         <v>197</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="12.75">
       <c r="A107" s="1" t="s">
         <v>199</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" ht="12.75">
       <c r="A108" s="1" t="s">
         <v>201</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" ht="12.75">
       <c r="A109" s="1" t="s">
         <v>203</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" ht="12.75">
       <c r="A110" s="1" t="s">
         <v>205</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" ht="12.75">
       <c r="A111" s="1" t="s">
         <v>207</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" ht="12.75">
       <c r="A112" s="1" t="s">
         <v>209</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" ht="12.75">
       <c r="A113" s="1" t="s">
         <v>211</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" ht="12.75">
       <c r="A114" s="1" t="s">
         <v>213</v>
       </c>
@@ -2165,7 +2171,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" ht="12.75">
       <c r="A115" s="1" t="s">
         <v>215</v>
       </c>
@@ -2173,7 +2179,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" ht="12.75">
       <c r="A116" s="1" t="s">
         <v>216</v>
       </c>
@@ -2181,7 +2187,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" ht="12.75">
       <c r="A117" s="1" t="s">
         <v>218</v>
       </c>
@@ -2189,7 +2195,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" ht="12.75">
       <c r="A118" s="1" t="s">
         <v>220</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" ht="12.75">
       <c r="A119" s="1" t="s">
         <v>222</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" ht="12.75">
       <c r="A120" s="1" t="s">
         <v>224</v>
       </c>
@@ -2213,7 +2219,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" ht="12.75">
       <c r="A121" s="1" t="s">
         <v>226</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" ht="12.75">
       <c r="A122" s="1" t="s">
         <v>228</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" ht="12.75">
       <c r="A123" s="1" t="s">
         <v>22</v>
       </c>
@@ -2237,7 +2243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" ht="12.75">
       <c r="A124" s="1" t="s">
         <v>20</v>
       </c>
@@ -2245,7 +2251,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" ht="12.75">
       <c r="A125" s="1" t="s">
         <v>16</v>
       </c>
@@ -2253,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" ht="12.75">
       <c r="A126" s="1" t="s">
         <v>24</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" ht="12.75">
       <c r="A127" s="1" t="s">
         <v>232</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" ht="12.75">
       <c r="A128" s="1" t="s">
         <v>232</v>
       </c>
@@ -2277,7 +2283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" ht="12.75">
       <c r="A129" s="1" t="s">
         <v>233</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" ht="12.75">
       <c r="A130" s="1" t="s">
         <v>234</v>
       </c>
@@ -2293,7 +2299,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" ht="12.75">
       <c r="A131" s="1" t="s">
         <v>96</v>
       </c>
@@ -2301,7 +2307,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" ht="12.75">
       <c r="A132" s="1" t="s">
         <v>235</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" ht="12.75">
       <c r="A133" s="1" t="s">
         <v>237</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" ht="12.75">
       <c r="A134" s="1" t="s">
         <v>233</v>
       </c>
@@ -2325,7 +2331,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" ht="12.75">
       <c r="A135" s="1" t="s">
         <v>234</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" ht="12.75">
       <c r="A136" s="1" t="s">
         <v>239</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" ht="12.75">
       <c r="A137" s="1" t="s">
         <v>241</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" ht="12.75">
       <c r="A138" s="1" t="s">
         <v>175</v>
       </c>
@@ -2357,7 +2363,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" ht="12.75">
       <c r="A139" s="1" t="s">
         <v>244</v>
       </c>
@@ -2365,7 +2371,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" ht="12.75">
       <c r="A140" s="1" t="s">
         <v>246</v>
       </c>
@@ -2373,7 +2379,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" ht="12.75">
       <c r="A141" s="1" t="s">
         <v>247</v>
       </c>
@@ -2381,7 +2387,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" ht="12.75">
       <c r="A142" s="1" t="s">
         <v>249</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" ht="12.75">
       <c r="A143" s="1" t="s">
         <v>251</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" ht="12.75">
       <c r="A144" s="2" t="s">
         <v>253</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" ht="12.75">
       <c r="A145" s="1" t="s">
         <v>255</v>
       </c>
@@ -2413,7 +2419,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" ht="12.75">
       <c r="A146" s="1" t="s">
         <v>257</v>
       </c>
@@ -2421,7 +2427,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" ht="12.75">
       <c r="A147" s="2" t="s">
         <v>259</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" ht="12.75">
       <c r="A148" s="1" t="s">
         <v>261</v>
       </c>
@@ -2437,7 +2443,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" ht="12.75">
       <c r="A149" s="1" t="s">
         <v>263</v>
       </c>
@@ -2445,7 +2451,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" ht="12.75">
       <c r="A150" s="1" t="s">
         <v>265</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" ht="12.75">
       <c r="A151" s="1" t="s">
         <v>266</v>
       </c>
@@ -2461,7 +2467,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" ht="12.75">
       <c r="A152" s="1" t="s">
         <v>267</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" ht="12.75">
       <c r="A153" s="1" t="s">
         <v>269</v>
       </c>
@@ -2477,7 +2483,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" ht="12.75">
       <c r="A154" s="1" t="s">
         <v>271</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" ht="12.75">
       <c r="A155" s="1" t="s">
         <v>273</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" ht="12.75">
       <c r="A156" s="1" t="s">
         <v>275</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" ht="12.75">
       <c r="A157" s="1" t="s">
         <v>266</v>
       </c>
@@ -2509,7 +2515,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" ht="12.75">
       <c r="A158" s="1" t="s">
         <v>278</v>
       </c>
@@ -2517,7 +2523,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" ht="12.75">
       <c r="A159" s="1" t="s">
         <v>280</v>
       </c>
@@ -2525,7 +2531,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" ht="12.75">
       <c r="A160" s="1" t="s">
         <v>282</v>
       </c>
@@ -2533,7 +2539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" ht="12.75">
       <c r="A161" s="1" t="s">
         <v>283</v>
       </c>
@@ -2541,7 +2547,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" ht="12.75">
       <c r="A162" s="1" t="s">
         <v>285</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" ht="12.75">
       <c r="A163" s="1" t="s">
         <v>287</v>
       </c>
@@ -2557,7 +2563,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" ht="12.75">
       <c r="A164" s="1" t="s">
         <v>171</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" ht="12.75">
       <c r="A165" s="1" t="s">
         <v>314</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" ht="12.75">
       <c r="A166" s="1" t="s">
         <v>291</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" ht="12.75">
       <c r="A167" s="1" t="s">
         <v>293</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" ht="12.75">
       <c r="A168" s="1" t="s">
         <v>295</v>
       </c>
@@ -2597,7 +2603,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" ht="12.75">
       <c r="A169" s="1" t="s">
         <v>315</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" ht="12.75">
       <c r="A170" s="1" t="s">
         <v>298</v>
       </c>
@@ -2613,7 +2619,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" ht="12.75">
       <c r="A171" s="1" t="s">
         <v>300</v>
       </c>
@@ -2621,7 +2627,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" ht="12.75">
       <c r="A172" s="1" t="s">
         <v>302</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" ht="12.75">
       <c r="A173" s="1" t="s">
         <v>304</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" ht="12.75">
       <c r="A174" s="1" t="s">
         <v>306</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" ht="12.75">
       <c r="A175" s="1" t="s">
         <v>308</v>
       </c>
@@ -2653,12 +2659,20 @@
         <v>309</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" ht="12.75">
       <c r="A176" s="1" t="s">
         <v>310</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>311</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A177" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B177" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- seperate ozone plots - update translation
</commit_message>
<xml_diff>
--- a/inst/extdata/label_translations.xlsx
+++ b/inst/extdata/label_translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Desktop\CREA Github\temp\china_co2\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994B070C-72AE-47DD-A3D3-734A37DCE720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF05886-5B40-427D-A918-D4FB84ED0027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="322">
   <si>
     <t>EN</t>
   </si>
@@ -980,6 +980,12 @@
   </si>
   <si>
     <t>日最大8小时平均第90百分位浓度</t>
+  </si>
+  <si>
+    <t>Monthly pollutant concentrations in provincial capitals (90th percentile)</t>
+  </si>
+  <si>
+    <t>省会城市月污染物浓度 (第90百分位)</t>
   </si>
 </sst>
 </file>
@@ -1253,10 +1259,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B178"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2689,6 +2695,14 @@
         <v>319</v>
       </c>
     </row>
+    <row r="179" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A179" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>